<commit_message>
Localization Language Get Daze！
Localization Language Get Daze！
</commit_message>
<xml_diff>
--- a/AAAGameData/Languages/ChineseSimplified.xlsx
+++ b/AAAGameData/Languages/ChineseSimplified.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\UnityProjects\UGF\AAAGameData\Languages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Fork Project\GF_X_Demo\AAAGameData\Languages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A27FB5F-DA67-4F4E-88AC-01C7EA57985C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A077E6-A276-42BD-A59E-85E74DDF8FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13875" yWindow="3075" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1" fullPrecision="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -25,37 +25,40 @@
     <author>Anonymous</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+        <r>
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">勾选锁定此行,锁定后将强制保留</t>
-        </d:r>
+          <t>勾选锁定此行,锁定后将强制保留</t>
+        </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
-        <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+        <r>
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">多语言Key</t>
-        </d:r>
+          <t>多语言Key</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
-        <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+        <r>
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
-          <t xml:space="preserve">多语言Value, 当值为空时, [一键翻译]会自动填充Value值</t>
-        </d:r>
+          <t>多语言Value, 当值为空时, [一键翻译]会自动填充Value值</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -116,9 +119,6 @@
     <t>MenuUIForm.Tips</t>
   </si>
   <si>
-    <t>点击开始</t>
-  </si>
-  <si>
     <t>Nothing</t>
   </si>
   <si>
@@ -249,17 +249,37 @@
   </si>
   <si>
     <t>解锁</t>
+  </si>
+  <si>
+    <t>空格键开始</t>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -282,11 +302,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -431,466 +452,6 @@
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14"/>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
@@ -905,15 +466,15 @@
           <xdr:row>1</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A1" id="1056">
+            <xdr:cNvPr id="1056" name="A1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -921,8 +482,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -935,7 +496,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -952,14 +513,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -991,15 +552,15 @@
           <xdr:row>2</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A2" id="1057">
+            <xdr:cNvPr id="1057" name="A2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1007,8 +568,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1021,7 +582,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1038,14 +599,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1077,15 +638,15 @@
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A3" id="1058">
+            <xdr:cNvPr id="1058" name="A3" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1093,8 +654,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1107,7 +668,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1124,14 +685,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1163,15 +724,15 @@
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A4" id="1059">
+            <xdr:cNvPr id="1059" name="A4" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1179,8 +740,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1193,7 +754,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1210,14 +771,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1249,15 +810,15 @@
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A5" id="1060">
+            <xdr:cNvPr id="1060" name="A5" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1265,8 +826,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1279,7 +840,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1296,14 +857,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1335,15 +896,15 @@
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A6" id="1061">
+            <xdr:cNvPr id="1061" name="A6" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1351,8 +912,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1365,7 +926,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1382,14 +943,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1421,15 +982,15 @@
           <xdr:row>7</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A7" id="1062">
+            <xdr:cNvPr id="1062" name="A7" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1437,8 +998,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1451,7 +1012,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1468,14 +1029,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1507,15 +1068,15 @@
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A8" id="1063">
+            <xdr:cNvPr id="1063" name="A8" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1523,8 +1084,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1537,7 +1098,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1554,14 +1115,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1590,18 +1151,18 @@
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>285750</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A9" id="1064">
+            <xdr:cNvPr id="1064" name="A9" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1064"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1609,8 +1170,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1623,7 +1184,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1640,14 +1201,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1679,15 +1240,15 @@
           <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A10" id="1065">
+            <xdr:cNvPr id="1065" name="A10" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1065"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1695,8 +1256,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1709,7 +1270,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1726,14 +1287,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1765,15 +1326,15 @@
           <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A11" id="1066">
+            <xdr:cNvPr id="1066" name="A11" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1066"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1781,8 +1342,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1795,7 +1356,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1812,14 +1373,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1851,15 +1412,15 @@
           <xdr:row>12</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A12" id="1067">
+            <xdr:cNvPr id="1067" name="A12" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1067"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1867,8 +1428,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1881,7 +1442,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1898,14 +1459,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1937,15 +1498,15 @@
           <xdr:row>13</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A13" id="1068">
+            <xdr:cNvPr id="1068" name="A13" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1068"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1953,8 +1514,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1967,7 +1528,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -1984,14 +1545,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2023,15 +1584,15 @@
           <xdr:row>14</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A14" id="1069">
+            <xdr:cNvPr id="1069" name="A14" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1069"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2039,8 +1600,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2053,7 +1614,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2070,14 +1631,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2109,15 +1670,15 @@
           <xdr:row>15</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A15" id="1070">
+            <xdr:cNvPr id="1070" name="A15" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1070"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2125,8 +1686,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2139,7 +1700,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2156,14 +1717,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2195,15 +1756,15 @@
           <xdr:row>16</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A16" id="1071">
+            <xdr:cNvPr id="1071" name="A16" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1071"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2211,8 +1772,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2225,7 +1786,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2242,14 +1803,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2281,15 +1842,15 @@
           <xdr:row>17</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A17" id="1072">
+            <xdr:cNvPr id="1072" name="A17" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1072"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2297,8 +1858,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2311,7 +1872,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2328,14 +1889,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2367,15 +1928,15 @@
           <xdr:row>18</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A18" id="1073">
+            <xdr:cNvPr id="1073" name="A18" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2383,8 +1944,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2397,7 +1958,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2414,14 +1975,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2453,15 +2014,15 @@
           <xdr:row>19</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A19" id="1074">
+            <xdr:cNvPr id="1074" name="A19" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1074"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2469,8 +2030,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2483,7 +2044,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2500,14 +2061,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2539,15 +2100,15 @@
           <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A20" id="1075">
+            <xdr:cNvPr id="1075" name="A20" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1075"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2555,8 +2116,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2569,7 +2130,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2586,14 +2147,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2625,15 +2186,15 @@
           <xdr:row>21</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A21" id="1076">
+            <xdr:cNvPr id="1076" name="A21" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1076"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2641,8 +2202,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2655,7 +2216,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2672,14 +2233,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2711,15 +2272,15 @@
           <xdr:row>22</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A22" id="1077">
+            <xdr:cNvPr id="1077" name="A22" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1077"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2727,8 +2288,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2741,7 +2302,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2758,14 +2319,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2797,15 +2358,15 @@
           <xdr:row>23</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A23" id="1078">
+            <xdr:cNvPr id="1078" name="A23" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1078"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2813,8 +2374,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2827,7 +2388,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2844,14 +2405,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2883,15 +2444,15 @@
           <xdr:row>24</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A24" id="1079">
+            <xdr:cNvPr id="1079" name="A24" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1079"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2899,8 +2460,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2913,7 +2474,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -2930,14 +2491,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2969,15 +2530,15 @@
           <xdr:row>25</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A25" id="1080">
+            <xdr:cNvPr id="1080" name="A25" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1080"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2985,8 +2546,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2999,7 +2560,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -3016,14 +2577,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3055,15 +2616,15 @@
           <xdr:row>26</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A26" id="1081">
+            <xdr:cNvPr id="1081" name="A26" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1081"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3071,8 +2632,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3085,7 +2646,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -3102,14 +2663,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3141,15 +2702,15 @@
           <xdr:row>27</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A27" id="1082">
+            <xdr:cNvPr id="1082" name="A27" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1082"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3157,8 +2718,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3171,7 +2732,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -3188,14 +2749,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3227,15 +2788,15 @@
           <xdr:row>28</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A28" id="1083">
+            <xdr:cNvPr id="1083" name="A28" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1083"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3243,8 +2804,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3257,7 +2818,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -3274,14 +2835,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3313,15 +2874,15 @@
           <xdr:row>29</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A29" id="1084">
+            <xdr:cNvPr id="1084" name="A29" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1084"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3329,8 +2890,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3343,7 +2904,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -3360,14 +2921,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3399,15 +2960,15 @@
           <xdr:row>30</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A30" id="1085">
+            <xdr:cNvPr id="1085" name="A30" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1085"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3415,8 +2976,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3429,7 +2990,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -3446,14 +3007,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3485,15 +3046,15 @@
           <xdr:row>31</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp macro="" textlink="" fLocksText="1">
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr hidden="1" name="A31" id="1086">
+            <xdr:cNvPr id="1086" name="A31" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1086"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3501,8 +3062,8 @@
           </xdr:nvSpPr>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off y="0" x="0"/>
-              <a:ext cy="0" cx="0"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3515,7 +3076,7 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
@@ -3532,14 +3093,14 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr upright="1" anchor="ctr" bIns="27432" rIns="27432" tIns="27432" lIns="27432" wrap="square" vertOverflow="clip"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr rtl="0" algn="l">
+              <a:pPr algn="l" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" baseline="0" strike="noStrike" u="none" i="0" b="0">
+                <a:rPr lang="zh-CN" altLang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3825,308 +3386,307 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.4074859619141" customWidth="1"/>
-    <col min="3" max="3" width="38.6902858189174" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="0" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1"/>
-      <c r="B11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="0" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
         <v>21</v>
       </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1"/>
-      <c r="B12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="0" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
         <v>23</v>
       </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="0" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" t="s">
         <v>25</v>
       </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1"/>
-      <c r="B14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="0" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
         <v>27</v>
       </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="0" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" t="s">
         <v>29</v>
       </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1"/>
-      <c r="B16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="0" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" t="s">
         <v>31</v>
       </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1"/>
-      <c r="B17" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="0" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" t="s">
         <v>33</v>
       </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="0" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" t="s">
         <v>35</v>
       </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1"/>
-      <c r="B19" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="0" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" t="s">
         <v>37</v>
       </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1"/>
-      <c r="B20" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="0" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" t="s">
         <v>39</v>
       </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1"/>
-      <c r="B21" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="0" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" t="s">
         <v>41</v>
       </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1"/>
-      <c r="B22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="0" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" t="s">
         <v>43</v>
       </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1"/>
-      <c r="B23" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="0" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" t="s">
         <v>45</v>
       </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1"/>
-      <c r="B24" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="0" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" t="s">
         <v>47</v>
       </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="0" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" t="s">
         <v>49</v>
       </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1"/>
-      <c r="B26" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="0" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" t="s">
         <v>51</v>
       </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1"/>
-      <c r="B27" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="0" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" t="s">
         <v>53</v>
       </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1"/>
-      <c r="B28" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="0" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" t="s">
         <v>55</v>
       </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1"/>
-      <c r="B29" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="0" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" t="s">
         <v>57</v>
       </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1"/>
-      <c r="B30" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="0" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1"/>
-      <c r="B31" s="0" t="s">
+      <c r="C31" t="s">
         <v>60</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1056" r:id="rId116" name="A1">
+            <control shapeId="1056" r:id="rId3" name="A1">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4146,9 +3706,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1057" r:id="rId117" name="A2">
+            <control shapeId="1057" r:id="rId4" name="A2">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4168,9 +3728,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1058" r:id="rId118" name="A3">
+            <control shapeId="1058" r:id="rId5" name="A3">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4190,9 +3750,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1059" r:id="rId119" name="A4">
+            <control shapeId="1059" r:id="rId6" name="A4">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4212,9 +3772,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1060" r:id="rId120" name="A5">
+            <control shapeId="1060" r:id="rId7" name="A5">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4234,9 +3794,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1061" r:id="rId121" name="A6">
+            <control shapeId="1061" r:id="rId8" name="A6">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4256,9 +3816,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1062" r:id="rId122" name="A7">
+            <control shapeId="1062" r:id="rId9" name="A7">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4278,9 +3838,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1063" r:id="rId123" name="A8">
+            <control shapeId="1063" r:id="rId10" name="A8">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4300,9 +3860,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1064" r:id="rId124" name="A9">
+            <control shapeId="1064" r:id="rId11" name="A9">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4314,17 +3874,17 @@
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>285750</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1065" r:id="rId125" name="A10">
+            <control shapeId="1065" r:id="rId12" name="A10">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4344,9 +3904,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1066" r:id="rId126" name="A11">
+            <control shapeId="1066" r:id="rId13" name="A11">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4366,9 +3926,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1067" r:id="rId127" name="A12">
+            <control shapeId="1067" r:id="rId14" name="A12">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4388,9 +3948,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1068" r:id="rId128" name="A13">
+            <control shapeId="1068" r:id="rId15" name="A13">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4410,9 +3970,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1069" r:id="rId129" name="A14">
+            <control shapeId="1069" r:id="rId16" name="A14">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4432,9 +3992,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1070" r:id="rId130" name="A15">
+            <control shapeId="1070" r:id="rId17" name="A15">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4454,9 +4014,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1071" r:id="rId131" name="A16">
+            <control shapeId="1071" r:id="rId18" name="A16">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4476,9 +4036,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1072" r:id="rId132" name="A17">
+            <control shapeId="1072" r:id="rId19" name="A17">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4498,9 +4058,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1073" r:id="rId133" name="A18">
+            <control shapeId="1073" r:id="rId20" name="A18">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4520,9 +4080,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1074" r:id="rId134" name="A19">
+            <control shapeId="1074" r:id="rId21" name="A19">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4542,9 +4102,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1075" r:id="rId135" name="A20">
+            <control shapeId="1075" r:id="rId22" name="A20">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4564,9 +4124,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1076" r:id="rId136" name="A21">
+            <control shapeId="1076" r:id="rId23" name="A21">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4586,9 +4146,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1077" r:id="rId137" name="A22">
+            <control shapeId="1077" r:id="rId24" name="A22">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4608,9 +4168,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1078" r:id="rId138" name="A23">
+            <control shapeId="1078" r:id="rId25" name="A23">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4630,9 +4190,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1079" r:id="rId139" name="A24">
+            <control shapeId="1079" r:id="rId26" name="A24">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4652,9 +4212,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1080" r:id="rId140" name="A25">
+            <control shapeId="1080" r:id="rId27" name="A25">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4674,9 +4234,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1081" r:id="rId141" name="A26">
+            <control shapeId="1081" r:id="rId28" name="A26">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4696,9 +4256,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1082" r:id="rId142" name="A27">
+            <control shapeId="1082" r:id="rId29" name="A27">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4718,9 +4278,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1083" r:id="rId143" name="A28">
+            <control shapeId="1083" r:id="rId30" name="A28">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4740,9 +4300,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1084" r:id="rId144" name="A29">
+            <control shapeId="1084" r:id="rId31" name="A29">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4762,9 +4322,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1085" r:id="rId145" name="A30">
+            <control shapeId="1085" r:id="rId32" name="A30">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4784,9 +4344,9 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
-        <mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1086" r:id="rId146" name="A31">
+            <control shapeId="1086" r:id="rId33" name="A31">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>